<commit_message>
Added hardware implementation for LTC2991s
</commit_message>
<xml_diff>
--- a/Documentation-Setup/LTC2991/LTC2991_Pin_Description.xlsx
+++ b/Documentation-Setup/LTC2991/LTC2991_Pin_Description.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CubeSat-WTC\Documentation-Setup\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34400" windowHeight="10110"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="10110"/>
   </bookViews>
   <sheets>
     <sheet name="LTC2991_Pin_Description_2-16-18" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="150">
   <si>
     <t>ADDR:</t>
   </si>
@@ -361,12 +356,120 @@
   </si>
   <si>
     <t>Joseph Sargent</t>
+  </si>
+  <si>
+    <t>DWN</t>
+  </si>
+  <si>
+    <t>Top Y+</t>
+  </si>
+  <si>
+    <t>Top Y-</t>
+  </si>
+  <si>
+    <t>J204</t>
+  </si>
+  <si>
+    <t>J205</t>
+  </si>
+  <si>
+    <t>J206</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Bridges go:</t>
+  </si>
+  <si>
+    <t>Values:</t>
+  </si>
+  <si>
+    <t>Bit Mapping:</t>
+  </si>
+  <si>
+    <t>Order:</t>
+  </si>
+  <si>
+    <t>J201</t>
+  </si>
+  <si>
+    <t>J202</t>
+  </si>
+  <si>
+    <t>J203</t>
+  </si>
+  <si>
+    <t>1 is:</t>
+  </si>
+  <si>
+    <t>*Silkscren is wrong</t>
+  </si>
+  <si>
+    <t>Bottom X-</t>
+  </si>
+  <si>
+    <t>J107</t>
+  </si>
+  <si>
+    <t>J111</t>
+  </si>
+  <si>
+    <t>J113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taken from back facing you. </t>
+  </si>
+  <si>
+    <t>Middle R</t>
+  </si>
+  <si>
+    <t>J110</t>
+  </si>
+  <si>
+    <t>J112</t>
+  </si>
+  <si>
+    <t>J114</t>
+  </si>
+  <si>
+    <t>Bottom Y+</t>
+  </si>
+  <si>
+    <t>Bottom Y-X+</t>
+  </si>
+  <si>
+    <t>Top L</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>J118</t>
+  </si>
+  <si>
+    <t>J119</t>
+  </si>
+  <si>
+    <t>J120</t>
+  </si>
+  <si>
+    <t>J115</t>
+  </si>
+  <si>
+    <t>J116</t>
+  </si>
+  <si>
+    <t>J117</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1257,7 +1360,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1265,21 +1368,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H106"/>
+  <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>73</v>
       </c>
@@ -1287,7 +1393,7 @@
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -1302,7 +1408,7 @@
       </c>
       <c r="F2" s="15"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>113</v>
       </c>
@@ -1312,7 +1418,7 @@
       </c>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>66</v>
       </c>
@@ -1327,7 +1433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1341,7 +1447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -1361,7 +1467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>68</v>
       </c>
@@ -1375,7 +1481,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>18</v>
       </c>
@@ -1389,8 +1495,14 @@
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>2</v>
       </c>
@@ -1404,7 +1516,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>3</v>
       </c>
@@ -1417,8 +1529,20 @@
       <c r="D10" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E10" t="s">
+        <v>125</v>
+      </c>
+      <c r="F10" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" t="s">
+        <v>127</v>
+      </c>
+      <c r="H10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>5</v>
       </c>
@@ -1431,8 +1555,20 @@
       <c r="D11" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -1445,8 +1581,14 @@
       <c r="D12" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
@@ -1460,7 +1602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
@@ -1474,8 +1616,20 @@
         <f t="shared" ref="D14" si="0">1/3</f>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E14" t="s">
+        <v>123</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
@@ -1488,8 +1642,20 @@
       <c r="D15" s="8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F15" t="s">
+        <v>114</v>
+      </c>
+      <c r="G15" t="s">
+        <v>114</v>
+      </c>
+      <c r="H15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1497,7 +1663,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>0</v>
       </c>
@@ -1511,7 +1677,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>68</v>
       </c>
@@ -1525,7 +1691,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>18</v>
       </c>
@@ -1539,8 +1705,14 @@
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E20" t="s">
+        <v>121</v>
+      </c>
+      <c r="F20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>2</v>
       </c>
@@ -1554,7 +1726,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>3</v>
       </c>
@@ -1567,8 +1739,23 @@
       <c r="D22" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E22" t="s">
+        <v>125</v>
+      </c>
+      <c r="F22" t="s">
+        <v>119</v>
+      </c>
+      <c r="G22" t="s">
+        <v>118</v>
+      </c>
+      <c r="H22" t="s">
+        <v>117</v>
+      </c>
+      <c r="I22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>5</v>
       </c>
@@ -1581,8 +1768,20 @@
       <c r="D23" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E23" t="s">
+        <v>124</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>7</v>
       </c>
@@ -1595,8 +1794,14 @@
       <c r="D24" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E24" t="s">
+        <v>129</v>
+      </c>
+      <c r="F24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>9</v>
       </c>
@@ -1610,7 +1815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>11</v>
       </c>
@@ -1623,8 +1828,20 @@
       <c r="D26" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E26" t="s">
+        <v>123</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>13</v>
       </c>
@@ -1638,8 +1855,20 @@
         <f t="shared" ref="D27" si="1">1/3</f>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E27" t="s">
+        <v>122</v>
+      </c>
+      <c r="F27" t="s">
+        <v>114</v>
+      </c>
+      <c r="G27" t="s">
+        <v>120</v>
+      </c>
+      <c r="H27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>66</v>
       </c>
@@ -1647,7 +1876,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1655,7 +1884,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>0</v>
       </c>
@@ -1669,7 +1898,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
         <v>68</v>
       </c>
@@ -1683,7 +1912,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>18</v>
       </c>
@@ -1696,8 +1925,17 @@
       <c r="D33" s="8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E33" t="s">
+        <v>121</v>
+      </c>
+      <c r="F33" t="s">
+        <v>131</v>
+      </c>
+      <c r="G33" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>2</v>
       </c>
@@ -1711,7 +1949,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>3</v>
       </c>
@@ -1724,8 +1962,23 @@
       <c r="D35" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E35" t="s">
+        <v>125</v>
+      </c>
+      <c r="F35" t="s">
+        <v>132</v>
+      </c>
+      <c r="G35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H35" t="s">
+        <v>134</v>
+      </c>
+      <c r="I35" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>5</v>
       </c>
@@ -1738,8 +1991,20 @@
       <c r="D36" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E36" t="s">
+        <v>124</v>
+      </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>7</v>
       </c>
@@ -1752,8 +2017,14 @@
       <c r="D37" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E37" t="s">
+        <v>129</v>
+      </c>
+      <c r="F37" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>9</v>
       </c>
@@ -1767,7 +2038,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>11</v>
       </c>
@@ -1780,8 +2051,20 @@
       <c r="D39" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E39" t="s">
+        <v>123</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>13</v>
       </c>
@@ -1794,8 +2077,20 @@
       <c r="D40" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E40" t="s">
+        <v>122</v>
+      </c>
+      <c r="F40" t="s">
+        <v>120</v>
+      </c>
+      <c r="G40" t="s">
+        <v>114</v>
+      </c>
+      <c r="H40" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>31</v>
       </c>
@@ -1803,7 +2098,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>0</v>
       </c>
@@ -1817,7 +2112,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>68</v>
       </c>
@@ -1831,7 +2126,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>18</v>
       </c>
@@ -1844,8 +2139,17 @@
       <c r="D45" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E45" t="s">
+        <v>121</v>
+      </c>
+      <c r="F45" t="s">
+        <v>140</v>
+      </c>
+      <c r="G45" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>2</v>
       </c>
@@ -1859,7 +2163,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>3</v>
       </c>
@@ -1872,8 +2176,23 @@
       <c r="D47" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E47" t="s">
+        <v>125</v>
+      </c>
+      <c r="F47" t="s">
+        <v>137</v>
+      </c>
+      <c r="G47" t="s">
+        <v>138</v>
+      </c>
+      <c r="H47" t="s">
+        <v>139</v>
+      </c>
+      <c r="I47" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>5</v>
       </c>
@@ -1886,8 +2205,20 @@
       <c r="D48" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E48" t="s">
+        <v>124</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>7</v>
       </c>
@@ -1900,8 +2231,14 @@
       <c r="D49" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E49" t="s">
+        <v>129</v>
+      </c>
+      <c r="F49" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>9</v>
       </c>
@@ -1915,7 +2252,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>11</v>
       </c>
@@ -1928,8 +2265,20 @@
       <c r="D51" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E51" t="s">
+        <v>123</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>13</v>
       </c>
@@ -1942,8 +2291,20 @@
       <c r="D52" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E52" t="s">
+        <v>122</v>
+      </c>
+      <c r="F52" t="s">
+        <v>114</v>
+      </c>
+      <c r="G52" t="s">
+        <v>120</v>
+      </c>
+      <c r="H52" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>31</v>
       </c>
@@ -1951,7 +2312,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>0</v>
       </c>
@@ -1965,7 +2326,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>68</v>
       </c>
@@ -1979,7 +2340,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>18</v>
       </c>
@@ -1992,8 +2353,14 @@
       <c r="D57" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E57" t="s">
+        <v>121</v>
+      </c>
+      <c r="F57" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>2</v>
       </c>
@@ -2007,7 +2374,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>3</v>
       </c>
@@ -2020,8 +2387,20 @@
       <c r="D59" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E59" t="s">
+        <v>125</v>
+      </c>
+      <c r="F59" t="s">
+        <v>147</v>
+      </c>
+      <c r="G59" t="s">
+        <v>148</v>
+      </c>
+      <c r="H59" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>5</v>
       </c>
@@ -2034,8 +2413,20 @@
       <c r="D60" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E60" t="s">
+        <v>124</v>
+      </c>
+      <c r="F60">
+        <v>2</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>7</v>
       </c>
@@ -2048,8 +2439,14 @@
       <c r="D61" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E61" t="s">
+        <v>129</v>
+      </c>
+      <c r="F61" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>9</v>
       </c>
@@ -2063,7 +2460,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>11</v>
       </c>
@@ -2076,8 +2473,20 @@
       <c r="D63" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E63" t="s">
+        <v>123</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>13</v>
       </c>
@@ -2090,8 +2499,20 @@
       <c r="D64" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E64" t="s">
+        <v>122</v>
+      </c>
+      <c r="F64" t="s">
+        <v>120</v>
+      </c>
+      <c r="G64" t="s">
+        <v>114</v>
+      </c>
+      <c r="H64" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>31</v>
       </c>
@@ -2099,7 +2520,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>0</v>
       </c>
@@ -2113,7 +2534,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>68</v>
       </c>
@@ -2127,7 +2548,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>18</v>
       </c>
@@ -2140,8 +2561,17 @@
       <c r="D69" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E69" t="s">
+        <v>121</v>
+      </c>
+      <c r="F69" t="s">
+        <v>141</v>
+      </c>
+      <c r="G69" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>2</v>
       </c>
@@ -2155,7 +2585,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>3</v>
       </c>
@@ -2168,8 +2598,23 @@
       <c r="D71" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E71" t="s">
+        <v>125</v>
+      </c>
+      <c r="F71" t="s">
+        <v>144</v>
+      </c>
+      <c r="G71" t="s">
+        <v>145</v>
+      </c>
+      <c r="H71" t="s">
+        <v>146</v>
+      </c>
+      <c r="I71" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>5</v>
       </c>
@@ -2182,8 +2627,20 @@
       <c r="D72" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E72" t="s">
+        <v>124</v>
+      </c>
+      <c r="F72">
+        <v>2</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>7</v>
       </c>
@@ -2196,8 +2653,14 @@
       <c r="D73" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E73" t="s">
+        <v>129</v>
+      </c>
+      <c r="F73" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>9</v>
       </c>
@@ -2211,7 +2674,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>11</v>
       </c>
@@ -2224,8 +2687,20 @@
       <c r="D75" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E75" t="s">
+        <v>123</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>13</v>
       </c>
@@ -2238,12 +2713,23 @@
       <c r="D76" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="H76" s="9"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E76" t="s">
+        <v>122</v>
+      </c>
+      <c r="F76" t="s">
+        <v>120</v>
+      </c>
+      <c r="G76" t="s">
+        <v>114</v>
+      </c>
+      <c r="H76" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H77" s="9"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
         <v>92</v>
       </c>
@@ -2252,7 +2738,7 @@
       <c r="D78" s="15"/>
       <c r="H78" s="9"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>80</v>
       </c>
@@ -2263,7 +2749,7 @@
       <c r="D79" s="14"/>
       <c r="H79" s="9"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>67</v>
       </c>
@@ -2274,7 +2760,7 @@
       <c r="D80" s="3"/>
       <c r="H80" s="9"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>0</v>
       </c>
@@ -2289,7 +2775,7 @@
       </c>
       <c r="H81" s="9"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>68</v>
       </c>
@@ -2304,7 +2790,7 @@
       </c>
       <c r="H82" s="9"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>18</v>
       </c>
@@ -2319,7 +2805,7 @@
       </c>
       <c r="H83" s="9"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>2</v>
       </c>
@@ -2334,7 +2820,7 @@
       </c>
       <c r="H84" s="9"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>3</v>
       </c>
@@ -2349,7 +2835,7 @@
       </c>
       <c r="H85" s="9"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>5</v>
       </c>
@@ -2364,7 +2850,7 @@
       </c>
       <c r="H86" s="9"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>7</v>
       </c>
@@ -2379,7 +2865,7 @@
       </c>
       <c r="H87" s="9"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>9</v>
       </c>
@@ -2394,7 +2880,7 @@
       </c>
       <c r="H88" s="9"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>11</v>
       </c>
@@ -2408,7 +2894,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>13</v>
       </c>
@@ -2422,13 +2908,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>

</xml_diff>

<commit_message>
Adding test bench code for LTC2991
</commit_message>
<xml_diff>
--- a/Documentation-Setup/LTC2991/LTC2991_Pin_Description.xlsx
+++ b/Documentation-Setup/LTC2991/LTC2991_Pin_Description.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="10110"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="10110"/>
   </bookViews>
   <sheets>
     <sheet name="LTC2991_Pin_Description_2-16-18" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="152">
   <si>
     <t>ADDR:</t>
   </si>
@@ -88,9 +88,6 @@
     <t>V_Stack_2</t>
   </si>
   <si>
-    <t>NTC_YZ</t>
-  </si>
-  <si>
     <t>TH-2-6+</t>
   </si>
   <si>
@@ -253,9 +250,6 @@
     <t>0V</t>
   </si>
   <si>
-    <t>2.5V</t>
-  </si>
-  <si>
     <t>Board:</t>
   </si>
   <si>
@@ -464,6 +458,18 @@
   </si>
   <si>
     <t>J117</t>
+  </si>
+  <si>
+    <t>3.3V(IO)</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>MPPT_Bus</t>
+  </si>
+  <si>
+    <t>5.9V</t>
   </si>
 </sst>
 </file>
@@ -1360,7 +1366,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1370,8 +1376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,7 +1393,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1395,39 +1401,39 @@
     </row>
     <row r="2" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="4">
         <v>43159</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3"/>
       <c r="E3" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="1"/>
       <c r="E4" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
@@ -1441,7 +1447,7 @@
         <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
@@ -1452,16 +1458,16 @@
         <v>0</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -1469,16 +1475,16 @@
     </row>
     <row r="7" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
@@ -1496,10 +1502,10 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="E8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
@@ -1510,10 +1516,10 @@
         <v>20</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
@@ -1530,16 +1536,16 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" t="s">
+        <v>124</v>
+      </c>
+      <c r="G10" t="s">
         <v>125</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>126</v>
-      </c>
-      <c r="G10" t="s">
-        <v>127</v>
-      </c>
-      <c r="H10" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
@@ -1556,7 +1562,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -1582,10 +1588,10 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
@@ -1617,7 +1623,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="E14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1637,22 +1643,22 @@
         <v>14</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>79</v>
+        <v>148</v>
       </c>
       <c r="D15" s="8">
         <v>0.5</v>
       </c>
       <c r="E15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
@@ -1668,27 +1674,27 @@
         <v>0</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
@@ -1706,10 +1712,10 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="E20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
@@ -1717,13 +1723,13 @@
         <v>2</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>24</v>
+        <v>149</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>91</v>
+        <v>71</v>
+      </c>
+      <c r="D21" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
@@ -1731,7 +1737,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>21</v>
@@ -1740,19 +1746,19 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
@@ -1760,7 +1766,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>21</v>
@@ -1769,7 +1775,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1786,7 +1792,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>21</v>
@@ -1795,10 +1801,10 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
@@ -1806,7 +1812,7 @@
         <v>9</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>21</v>
@@ -1820,16 +1826,16 @@
         <v>11</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>24</v>
+        <v>149</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>91</v>
+        <v>71</v>
+      </c>
+      <c r="D26" s="8">
+        <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1846,7 +1852,7 @@
         <v>13</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>19</v>
@@ -1856,32 +1862,32 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="E27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F27" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G27" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H27" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
         <v>31</v>
-      </c>
-      <c r="B30" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
@@ -1889,110 +1895,110 @@
         <v>0</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D32" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B33" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="D33" s="8">
         <v>0.5</v>
       </c>
       <c r="E33" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F33" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G33" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="6">
+        <v>33</v>
+      </c>
+      <c r="D34" s="8">
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35" s="6">
+        <v>33</v>
+      </c>
+      <c r="D35" s="8">
         <v>0.5</v>
       </c>
       <c r="E35" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F35" t="s">
+        <v>130</v>
+      </c>
+      <c r="G35" t="s">
+        <v>131</v>
+      </c>
+      <c r="H35" t="s">
         <v>132</v>
       </c>
-      <c r="G35" t="s">
+      <c r="I35" t="s">
         <v>133</v>
       </c>
-      <c r="H35" t="s">
-        <v>134</v>
-      </c>
-      <c r="I35" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D36" s="6">
+        <v>74</v>
+      </c>
+      <c r="D36" s="8">
         <v>0.5</v>
       </c>
       <c r="E36" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F36">
         <v>2</v>
@@ -2004,55 +2010,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D37" s="6">
+        <v>74</v>
+      </c>
+      <c r="D37" s="8">
         <v>0.5</v>
       </c>
       <c r="E37" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F37" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D38" s="6">
+        <v>33</v>
+      </c>
+      <c r="D38" s="8">
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D39" s="6">
+        <v>33</v>
+      </c>
+      <c r="D39" s="8">
         <v>0.5</v>
       </c>
       <c r="E39" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -2064,38 +2070,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B40" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E40" t="s">
+        <v>120</v>
+      </c>
+      <c r="F40" t="s">
+        <v>118</v>
+      </c>
+      <c r="G40" t="s">
+        <v>112</v>
+      </c>
+      <c r="H40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" t="s">
         <v>41</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D40" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="E40" t="s">
-        <v>122</v>
-      </c>
-      <c r="F40" t="s">
-        <v>120</v>
-      </c>
-      <c r="G40" t="s">
-        <v>114</v>
-      </c>
-      <c r="H40" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>31</v>
-      </c>
-      <c r="B42" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2103,27 +2109,27 @@
         <v>0</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C43">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="C44" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="D44" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2131,22 +2137,22 @@
         <v>18</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D45" s="6">
+        <v>75</v>
+      </c>
+      <c r="D45" s="8">
         <v>0.5</v>
       </c>
       <c r="E45" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F45" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G45" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2154,12 +2160,12 @@
         <v>2</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D46" s="6">
+        <v>75</v>
+      </c>
+      <c r="D46" s="8">
         <v>0.5</v>
       </c>
     </row>
@@ -2168,28 +2174,28 @@
         <v>3</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D47" s="6">
+        <v>75</v>
+      </c>
+      <c r="D47" s="8">
         <v>0.5</v>
       </c>
       <c r="E47" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F47" t="s">
+        <v>135</v>
+      </c>
+      <c r="G47" t="s">
+        <v>136</v>
+      </c>
+      <c r="H47" t="s">
         <v>137</v>
       </c>
-      <c r="G47" t="s">
-        <v>138</v>
-      </c>
-      <c r="H47" t="s">
-        <v>139</v>
-      </c>
       <c r="I47" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2197,16 +2203,16 @@
         <v>5</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D48" s="6">
+        <v>75</v>
+      </c>
+      <c r="D48" s="8">
         <v>0.5</v>
       </c>
       <c r="E48" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F48">
         <v>2</v>
@@ -2223,19 +2229,19 @@
         <v>7</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D49" s="6">
+        <v>74</v>
+      </c>
+      <c r="D49" s="8">
         <v>0.5</v>
       </c>
       <c r="E49" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F49" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -2243,12 +2249,12 @@
         <v>9</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D50" s="6">
+        <v>76</v>
+      </c>
+      <c r="D50" s="8">
         <v>0.5</v>
       </c>
     </row>
@@ -2257,16 +2263,16 @@
         <v>11</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D51" s="6">
+        <v>75</v>
+      </c>
+      <c r="D51" s="8">
         <v>0.5</v>
       </c>
       <c r="E51" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -2283,33 +2289,33 @@
         <v>13</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D52" s="6">
+        <v>75</v>
+      </c>
+      <c r="D52" s="8">
         <v>0.5</v>
       </c>
       <c r="E52" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F52" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G52" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H52" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2317,27 +2323,27 @@
         <v>0</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C55">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="C56" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="D56" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -2345,19 +2351,19 @@
         <v>18</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D57" s="6">
+        <v>75</v>
+      </c>
+      <c r="D57" s="8">
         <v>0.5</v>
       </c>
       <c r="E57" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F57" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -2365,12 +2371,12 @@
         <v>2</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D58" s="6">
+        <v>75</v>
+      </c>
+      <c r="D58" s="8">
         <v>0.5</v>
       </c>
     </row>
@@ -2379,25 +2385,25 @@
         <v>3</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D59" s="6">
+        <v>75</v>
+      </c>
+      <c r="D59" s="8">
         <v>0.5</v>
       </c>
       <c r="E59" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F59" t="s">
+        <v>145</v>
+      </c>
+      <c r="G59" t="s">
+        <v>146</v>
+      </c>
+      <c r="H59" t="s">
         <v>147</v>
-      </c>
-      <c r="G59" t="s">
-        <v>148</v>
-      </c>
-      <c r="H59" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -2405,16 +2411,16 @@
         <v>5</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D60" s="6">
+        <v>75</v>
+      </c>
+      <c r="D60" s="8">
         <v>0.5</v>
       </c>
       <c r="E60" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F60">
         <v>2</v>
@@ -2431,19 +2437,19 @@
         <v>7</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D61" s="6">
+        <v>75</v>
+      </c>
+      <c r="D61" s="8">
         <v>0.5</v>
       </c>
       <c r="E61" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F61" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -2451,12 +2457,12 @@
         <v>9</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D62" s="6">
+        <v>75</v>
+      </c>
+      <c r="D62" s="8">
         <v>0.5</v>
       </c>
     </row>
@@ -2465,16 +2471,16 @@
         <v>11</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D63" s="6">
+        <v>75</v>
+      </c>
+      <c r="D63" s="8">
         <v>0.5</v>
       </c>
       <c r="E63" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -2491,33 +2497,33 @@
         <v>13</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>91</v>
+        <v>77</v>
+      </c>
+      <c r="D64" s="8">
+        <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F64" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G64" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H64" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B66" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -2525,27 +2531,27 @@
         <v>0</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C67">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="C68" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="D68" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -2553,22 +2559,22 @@
         <v>18</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D69" s="6">
+        <v>74</v>
+      </c>
+      <c r="D69" s="8">
         <v>0.5</v>
       </c>
       <c r="E69" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F69" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G69" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -2576,12 +2582,12 @@
         <v>2</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D70" s="6">
+        <v>74</v>
+      </c>
+      <c r="D70" s="8">
         <v>0.5</v>
       </c>
     </row>
@@ -2590,28 +2596,28 @@
         <v>3</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D71" s="6">
+        <v>74</v>
+      </c>
+      <c r="D71" s="8">
         <v>0.5</v>
       </c>
       <c r="E71" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F71" t="s">
+        <v>142</v>
+      </c>
+      <c r="G71" t="s">
+        <v>143</v>
+      </c>
+      <c r="H71" t="s">
         <v>144</v>
       </c>
-      <c r="G71" t="s">
-        <v>145</v>
-      </c>
-      <c r="H71" t="s">
-        <v>146</v>
-      </c>
       <c r="I71" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -2619,16 +2625,16 @@
         <v>5</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D72" s="6">
+        <v>33</v>
+      </c>
+      <c r="D72" s="8">
         <v>0.5</v>
       </c>
       <c r="E72" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F72">
         <v>2</v>
@@ -2645,19 +2651,19 @@
         <v>7</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D73" s="6">
+        <v>33</v>
+      </c>
+      <c r="D73" s="8">
         <v>0.5</v>
       </c>
       <c r="E73" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F73" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -2665,13 +2671,13 @@
         <v>9</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>91</v>
+        <v>77</v>
+      </c>
+      <c r="D74" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -2679,16 +2685,16 @@
         <v>11</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>91</v>
+        <v>77</v>
+      </c>
+      <c r="D75" s="8">
+        <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F75">
         <v>1</v>
@@ -2705,25 +2711,25 @@
         <v>13</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>59</v>
+        <v>150</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>91</v>
+        <v>151</v>
+      </c>
+      <c r="D76" s="8">
+        <v>0.5</v>
       </c>
       <c r="E76" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F76" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G76" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H76" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -2731,7 +2737,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B78" s="15"/>
       <c r="C78" s="15"/>
@@ -2740,10 +2746,10 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C79" s="14"/>
       <c r="D79" s="14"/>
@@ -2751,10 +2757,10 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
@@ -2765,28 +2771,28 @@
         <v>0</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C81">
         <v>7</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H81" s="9"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B82" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="C82" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C82" s="6" t="s">
+      <c r="D82" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="H82" s="9"/>
     </row>
@@ -2795,13 +2801,13 @@
         <v>18</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C83" s="6">
         <v>12</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H83" s="9"/>
     </row>
@@ -2810,13 +2816,13 @@
         <v>2</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C84" s="6">
         <v>12</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H84" s="9"/>
     </row>
@@ -2825,13 +2831,13 @@
         <v>3</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C85" s="6">
         <v>12</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H85" s="9"/>
     </row>
@@ -2840,13 +2846,13 @@
         <v>5</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C86" s="6">
         <v>7.2</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H86" s="9"/>
     </row>
@@ -2855,13 +2861,13 @@
         <v>7</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C87" s="6">
         <v>5</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H87" s="9"/>
     </row>
@@ -2870,13 +2876,13 @@
         <v>9</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C88" s="6">
         <v>5</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H88" s="9"/>
     </row>
@@ -2885,13 +2891,13 @@
         <v>11</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C89" s="6">
         <v>5</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -2899,13 +2905,13 @@
         <v>13</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C90" s="6">
         <v>5</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>